<commit_message>
added stop activity also
</commit_message>
<xml_diff>
--- a/Udemy-BryanLamb-Level2/BuildSimpleRobot-Finish/Customers.xlsx
+++ b/Udemy-BryanLamb-Level2/BuildSimpleRobot-Finish/Customers.xlsx
@@ -3,7 +3,7 @@
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F432EC1B-AFC2-4804-A396-E3A4BB9244C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD57F585-2EA2-46CC-8E25-6B5B2604F09B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -224,9 +224,8 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="4">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -234,11 +233,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="6">
+  <x:cellXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -248,8 +246,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
-  <x:cellStyles count="2">
-    <x:cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -533,257 +530,254 @@
   <x:dimension ref="A1:D12"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A14" sqref="A14 A14:A14"/>
+      <x:selection activeCell="E1" sqref="E1 E1:G1048576"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="10.710938" style="4" customWidth="1"/>
-    <x:col min="2" max="2" width="11.285156" style="4" customWidth="1"/>
-    <x:col min="3" max="3" width="4" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="21.285156" style="4" customWidth="1"/>
+    <x:col min="1" max="1" width="10.710938" style="3" customWidth="1"/>
+    <x:col min="2" max="2" width="11.285156" style="3" customWidth="1"/>
+    <x:col min="3" max="3" width="4" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="21.285156" style="3" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="4" t="s">
+      <x:c r="A1" s="3" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="4" t="s">
+      <x:c r="B1" s="3" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="4" t="s">
+      <x:c r="C1" s="3" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="4" t="s">
+      <x:c r="D1" s="3" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="4" t="s">
+      <x:c r="E1" s="3" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="4" t="s">
+      <x:c r="F1" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="4" t="s">
+      <x:c r="A2" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B2" s="4" t="s">
+      <x:c r="B2" s="3" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C2" s="4" t="n">
+      <x:c r="C2" s="3" t="n">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="D2" s="5" t="s">
+      <x:c r="D2" s="4" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E2" s="4" t="s">
+      <x:c r="E2" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F2" s="4" t="s">
+      <x:c r="F2" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="4" t="s">
+      <x:c r="A3" s="3" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B3" s="4" t="s">
+      <x:c r="B3" s="3" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="C3" s="4" t="n">
+      <x:c r="C3" s="3" t="n">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="D3" s="5" t="s">
+      <x:c r="D3" s="4" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E3" s="4" t="s">
+      <x:c r="E3" s="3" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="F3" s="4" t="s">
+      <x:c r="F3" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="4" t="s">
+      <x:c r="A4" s="3" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="B4" s="4" t="s">
+      <x:c r="B4" s="3" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="C4" s="4" t="n">
+      <x:c r="C4" s="3" t="n">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D4" s="5" t="s">
+      <x:c r="D4" s="4" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="E4" s="4" t="s">
+      <x:c r="E4" s="3" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F4" s="4" t="s">
+      <x:c r="F4" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="4" t="s">
+      <x:c r="A5" s="3" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="B5" s="4" t="s">
+      <x:c r="B5" s="3" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="C5" s="4" t="s">
+      <x:c r="C5" s="3" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="D5" s="5" t="s">
+      <x:c r="D5" s="4" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="E5" s="4" t="s">
+      <x:c r="E5" s="3" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="F5" s="4" t="s">
+      <x:c r="F5" s="3" t="s">
         <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="4" t="s">
+      <x:c r="A6" s="3" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B6" s="4" t="s">
+      <x:c r="B6" s="3" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C6" s="4" t="n">
+      <x:c r="C6" s="3" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="D6" s="5" t="s">
+      <x:c r="D6" s="4" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="E6" s="4" t="s">
+      <x:c r="E6" s="3" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="F6" s="4" t="s">
+      <x:c r="F6" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="4" t="s">
+      <x:c r="A7" s="3" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="B7" s="4" t="s">
+      <x:c r="B7" s="3" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="C7" s="4" t="n">
+      <x:c r="C7" s="3" t="n">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="D7" s="5" t="s">
+      <x:c r="D7" s="4" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="E7" s="4" t="s">
+      <x:c r="E7" s="3" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="F7" s="4" t="s">
+      <x:c r="F7" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="4" t="s">
+      <x:c r="A8" s="3" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="B8" s="4" t="s">
+      <x:c r="B8" s="3" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="C8" s="4" t="n">
+      <x:c r="C8" s="3" t="n">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="D8" s="4" t="s"/>
-      <x:c r="E8" s="4" t="s">
+      <x:c r="D8" s="3" t="s"/>
+      <x:c r="E8" s="3" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="F8" s="4" t="s">
+      <x:c r="F8" s="3" t="s">
         <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="4" t="s">
+      <x:c r="A9" s="3" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="B9" s="4" t="s">
+      <x:c r="B9" s="3" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C9" s="4" t="n">
+      <x:c r="C9" s="3" t="n">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="D9" s="5" t="s">
+      <x:c r="D9" s="4" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E9" s="4" t="s">
+      <x:c r="E9" s="3" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="F9" s="4" t="s">
+      <x:c r="F9" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="4" t="s">
+      <x:c r="A10" s="3" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="B10" s="4" t="s">
+      <x:c r="B10" s="3" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="C10" s="4" t="n">
+      <x:c r="C10" s="3" t="n">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D10" s="5" t="s">
+      <x:c r="D10" s="4" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="E10" s="4" t="s">
+      <x:c r="E10" s="3" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="F10" s="4" t="s">
+      <x:c r="F10" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="4" t="s">
+      <x:c r="A11" s="3" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="B11" s="4" t="s">
+      <x:c r="B11" s="3" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="C11" s="4" t="n">
+      <x:c r="C11" s="3" t="n">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="D11" s="5" t="s">
+      <x:c r="D11" s="4" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="E11" s="4" t="s">
+      <x:c r="E11" s="3" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="F11" s="4" t="s">
+      <x:c r="F11" s="3" t="s">
         <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="4" t="s">
+      <x:c r="A12" s="3" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="B12" s="4" t="s">
+      <x:c r="B12" s="3" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="C12" s="4" t="n">
+      <x:c r="C12" s="3" t="n">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D12" s="5" t="s">
+      <x:c r="D12" s="4" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="E12" s="4" t="s">
+      <x:c r="E12" s="3" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="F12" s="4" t="s">
+      <x:c r="F12" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
-    </x:row>
-    <x:row r="14" spans="1:6">
-      <x:c r="A14" s="4" t="s"/>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>

</xml_diff>